<commit_message>
inserindo uma função  recursiva
</commit_message>
<xml_diff>
--- a/Base.xlsx
+++ b/Base.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\projeto_dennis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3eb1ecf9c67a8e3f/Área de Trabalho/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410F1210-DC01-42D4-BFCC-01639D4939C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{A177A38C-AF36-4FA8-9D3F-2D65032C2872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E97E6F26-2D63-42C6-A590-6BF0D20BC76C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1237BF47-BEE5-4097-9DF6-CA855100B5B1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1237BF47-BEE5-4097-9DF6-CA855100B5B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -446,21 +446,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FD6F9F-452E-4BCD-86E2-195603ABEFAA}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8:H43"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -474,220 +474,124 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1028791230</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1022877647</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>1012248698</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>1031263052</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>1029772220</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>1032926411</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>1009297179</v>
-      </c>
-      <c r="H8" s="1">
-        <v>1014748752</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>1008299011</v>
-      </c>
-      <c r="H9" s="1">
-        <v>1004144145</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H10" s="1">
-        <v>1000073570</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H11" s="1">
-        <v>1029661021</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H12" s="1">
-        <v>1001378587</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H13" s="1">
-        <v>1017300884</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H14" s="1">
-        <v>1002987935</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H15" s="1">
-        <v>1004040560</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H16" s="1">
-        <v>1022126676</v>
-      </c>
-    </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H17" s="1">
-        <v>1010333302</v>
-      </c>
-    </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H18" s="1">
-        <v>1010661776</v>
-      </c>
-    </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H19" s="1">
-        <v>1025356702</v>
-      </c>
-    </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H20" s="1">
-        <v>1002986440</v>
-      </c>
-    </row>
-    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H21" s="1">
-        <v>1017989904</v>
-      </c>
-    </row>
-    <row r="22" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H22" s="1">
-        <v>1017435011</v>
-      </c>
-    </row>
-    <row r="23" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H23" s="1">
-        <v>1018813389</v>
-      </c>
-    </row>
-    <row r="24" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H24" s="1">
-        <v>1024985650</v>
-      </c>
-    </row>
-    <row r="25" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H25" s="1">
-        <v>1004870172</v>
-      </c>
-    </row>
-    <row r="26" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H26" s="1">
-        <v>1028606300</v>
-      </c>
-    </row>
-    <row r="27" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H27" s="1">
-        <v>1025582532</v>
-      </c>
-    </row>
-    <row r="28" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H28" s="1">
-        <v>1026821670</v>
-      </c>
-    </row>
-    <row r="29" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H29" s="1">
-        <v>1017410027</v>
-      </c>
-    </row>
-    <row r="30" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H30" s="1">
-        <v>1015110220</v>
-      </c>
-    </row>
-    <row r="31" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H31" s="1">
-        <v>2804912668</v>
-      </c>
-    </row>
-    <row r="32" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H32" s="1">
-        <v>1025774296</v>
-      </c>
-    </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H33" s="1">
-        <v>1008380358</v>
-      </c>
-    </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H34" s="1">
-        <v>1009862020</v>
-      </c>
-    </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H35" s="1">
-        <v>1007272535</v>
-      </c>
-    </row>
-    <row r="36" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H36" s="1">
-        <v>1030665599</v>
-      </c>
-    </row>
-    <row r="37" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H37" s="1">
-        <v>1011859260</v>
-      </c>
-    </row>
-    <row r="38" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H38" s="1">
-        <v>1020589970</v>
-      </c>
-    </row>
-    <row r="39" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H39" s="1">
-        <v>2840984274</v>
-      </c>
-    </row>
-    <row r="40" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H40" s="1">
-        <v>1062918212</v>
-      </c>
-    </row>
-    <row r="41" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H41" s="1">
-        <v>1017737522</v>
-      </c>
-    </row>
-    <row r="42" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H42" s="1">
-        <v>1019029398</v>
-      </c>
-    </row>
-    <row r="43" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H43" s="1">
-        <v>1017737522</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2896917513</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2894373354</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2897658856</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1104572866</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2890563329</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2895484893</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2894980544</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2894374164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2897770710</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2895486560</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2894345342</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2894322601</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2895490354</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>2894348945</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2896429268</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>2854414971</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2897782123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2896925346</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2896103397</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2885673472</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>2894978957</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2894758639</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>2894773980</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>1113901516</v>
       </c>
     </row>
   </sheetData>

</xml_diff>